<commit_message>
ke: update FTS form
</commit_message>
<xml_diff>
--- a/LF/PreTAS/Kenya/ke_lf_pretas_3_resultat_fts_202203.xlsx
+++ b/LF/PreTAS/Kenya/ke_lf_pretas_3_resultat_fts_202203.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12240" tabRatio="500"/>
+    <workbookView windowWidth="28800" windowHeight="12240" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -400,37 +400,37 @@
     <t>why_invalid</t>
   </si>
   <si>
-    <t>Absence.de.ligne.temoin/controle</t>
+    <t>Absence.of.control.line</t>
   </si>
   <si>
     <t>Absence of control line</t>
   </si>
   <si>
-    <t>Ligne.temoin.discontinue/partielle</t>
+    <t>Broken/partial.control.line</t>
   </si>
   <si>
     <t>Broken/partial control line</t>
   </si>
   <si>
-    <t>Difficulte.d’absorption.d’echantillon</t>
+    <t>Difficulty.of.absorbing.sample</t>
   </si>
   <si>
     <t>Difficulty of absorbing sample</t>
   </si>
   <si>
-    <t>Difficulte.de.migration.d’echantillon</t>
+    <t>Difficulty.of.migrating.sample</t>
   </si>
   <si>
     <t>Difficulty of migrating sample</t>
   </si>
   <si>
-    <t>Trace.de.sang.persiste.(sang.reste.sur.la.bandelette/a.obscurci.les.lignes)</t>
+    <t>Trace.of.blood.persists</t>
   </si>
   <si>
     <t>Trace of blood persists</t>
   </si>
   <si>
-    <t>Insuffisance.du.volume.de.sang.du.a.la.pipette</t>
+    <t>Insufficient.blood.volume.due.to.pipette</t>
   </si>
   <si>
     <t>Insufficient blood volume due to pipette</t>
@@ -1688,12 +1688,12 @@
   <sheetPr/>
   <dimension ref="A1:N31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="D13" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A10" sqref="A10"/>
+      <selection pane="bottomRight" activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25"/>
@@ -2427,10 +2427,10 @@
   <sheetPr/>
   <dimension ref="A1:F328"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C14" sqref="C14:C18"/>
+      <selection pane="bottomLeft" activeCell="B7" sqref="B7:B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" outlineLevelCol="5"/>

</xml_diff>

<commit_message>
sn: add senegal document
</commit_message>
<xml_diff>
--- a/LF/PreTAS/Kenya/ke_lf_pretas_3_resultat_fts_202203.xlsx
+++ b/LF/PreTAS/Kenya/ke_lf_pretas_3_resultat_fts_202203.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12390" tabRatio="500"/>
+    <workbookView windowWidth="28800" windowHeight="12330" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="170">
   <si>
     <t>type</t>
   </si>
@@ -529,10 +529,10 @@
     <t xml:space="preserve">allow_choice_duplicates </t>
   </si>
   <si>
-    <t>3. Kenya - Pre TAS LF FTS Results Form V4</t>
-  </si>
-  <si>
-    <t>ke_lf_pretas_3_resultat_fts_202203_v4</t>
+    <t>3. Kenya - Pre TAS LF FTS Results Form V4.1</t>
+  </si>
+  <si>
+    <t>ke_lf_pretas_3_resultat_fts_202203_v4_1</t>
   </si>
   <si>
     <t>English</t>
@@ -544,9 +544,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="178" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -606,14 +606,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -621,16 +613,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -652,31 +652,30 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -690,8 +689,22 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="11"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -705,32 +718,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -739,6 +731,14 @@
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -763,7 +763,145 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -775,67 +913,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -847,61 +925,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -913,31 +937,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -966,6 +966,71 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -990,56 +1055,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -1048,160 +1063,145 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="16" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="25" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1625,11 +1625,11 @@
   <dimension ref="A1:N30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A8" sqref="$A8:$XFD8"/>
+      <selection pane="bottomRight" activeCell="A14" sqref="$A14:$XFD14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25"/>
@@ -1985,7 +1985,7 @@
     </row>
     <row r="14" s="3" customFormat="1" spans="1:13">
       <c r="A14" s="17" t="s">
-        <v>14</v>
+        <v>43</v>
       </c>
       <c r="B14" s="22" t="s">
         <v>61</v>
@@ -1997,13 +1997,9 @@
       <c r="E14" s="27"/>
       <c r="F14" s="18"/>
       <c r="G14" s="19"/>
-      <c r="H14" s="18" t="s">
-        <v>49</v>
-      </c>
+      <c r="H14" s="18"/>
       <c r="I14" s="18"/>
-      <c r="J14" s="27" t="s">
-        <v>18</v>
-      </c>
+      <c r="J14" s="27"/>
       <c r="K14" s="27"/>
       <c r="L14" s="27"/>
       <c r="M14" s="17"/>
@@ -2131,7 +2127,7 @@
     </row>
     <row r="20" s="3" customFormat="1" spans="1:13">
       <c r="A20" s="17" t="s">
-        <v>14</v>
+        <v>43</v>
       </c>
       <c r="B20" s="24" t="s">
         <v>81</v>
@@ -2147,9 +2143,7 @@
         <v>80</v>
       </c>
       <c r="I20" s="17"/>
-      <c r="J20" s="27" t="s">
-        <v>18</v>
-      </c>
+      <c r="J20" s="27"/>
       <c r="K20" s="17"/>
       <c r="L20" s="17"/>
       <c r="M20" s="17"/>
@@ -4388,7 +4382,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" outlineLevelRow="1" outlineLevelCol="3"/>

</xml_diff>